<commit_message>
Fondo di emergenza investito
</commit_message>
<xml_diff>
--- a/2023-10-02 Fondo di emergenza investito/2023-10-02 fondo di emergenza investito.xlsx
+++ b/2023-10-02 Fondo di emergenza investito/2023-10-02 fondo di emergenza investito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guifo\Il mio Drive\Content creation\Video YouTube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27AE035-1B7B-4627-9EEC-90F3CDD496CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD224D9C-C416-4E52-BB17-E26522C3929D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{6E0A3B31-7E40-4EC6-A308-0B231696AC3F}"/>
   </bookViews>
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>